<commit_message>
bug @Author : Alex
</commit_message>
<xml_diff>
--- a/04 Test Case/故障对应报告.xlsx
+++ b/04 Test Case/故障对应报告.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView xWindow="3270" yWindow="-315" windowWidth="14310" windowHeight="9690" activeTab="1"/>
@@ -14,8 +14,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">故障对应报告!$B$15:$I$15</definedName>
     <definedName name="createtime">版本履历!$E$4:$F$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">版本履历!$A$2:J34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">故障对应报告!$A$1:$I$17</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">版本履历!$A$2:J34</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">故障对应报告!$4:$5</definedName>
     <definedName name="project">版本履历!$B$4:$B$5</definedName>
     <definedName name="title" localSheetId="0">版本履历!$B$4:$I$5</definedName>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>完成时间</t>
   </si>
@@ -101,9 +101,6 @@
     <t>点击搜索按钮时，页面出了两层搜索框和搜索按钮</t>
   </si>
   <si>
-    <t>首页的图片游戏，显示变形</t>
-  </si>
-  <si>
     <t>一周热榜和最新下拉的时候没有翻页</t>
   </si>
   <si>
@@ -121,17 +118,26 @@
   </si>
   <si>
     <t>日志Logger wogamecenter_info.log 不准确</t>
+  </si>
+  <si>
+    <t>首页的图片游戏，显示变形
+Banner没有撑满屏幕</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>有些游戏的图标没有显示出来</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yy/m/d"/>
-    <numFmt numFmtId="165" formatCode="yy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="yy/m/d"/>
+    <numFmt numFmtId="177" formatCode="yy/mm/dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <name val="ＭＳ 明朝"/>
@@ -215,6 +221,12 @@
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -406,13 +418,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -424,11 +436,44 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -436,90 +481,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="標準_Sheet1" xfId="3"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="標準_Sheet1" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1016,7 +1033,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -1025,322 +1042,334 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="6" style="35" customWidth="1"/>
-    <col min="3" max="3" width="8" style="35" customWidth="1"/>
-    <col min="4" max="4" width="10" style="35" customWidth="1"/>
-    <col min="5" max="9" width="8" style="35" customWidth="1"/>
-    <col min="10" max="10" width="1.625" style="35" customWidth="1"/>
-    <col min="11" max="12" width="8" style="35" customWidth="1"/>
-    <col min="13" max="16384" width="8" style="35"/>
+    <col min="1" max="1" width="1.625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="6" style="23" customWidth="1"/>
+    <col min="3" max="3" width="8" style="23" customWidth="1"/>
+    <col min="4" max="4" width="10" style="23" customWidth="1"/>
+    <col min="5" max="9" width="8" style="23" customWidth="1"/>
+    <col min="10" max="10" width="1.625" style="23" customWidth="1"/>
+    <col min="11" max="12" width="8" style="23" customWidth="1"/>
+    <col min="13" max="16384" width="8" style="23"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="26" customFormat="1" ht="19.5" customHeight="1">
-      <c r="B2" s="25" t="s">
+    <row r="2" spans="2:9" s="16" customFormat="1" ht="19.5" customHeight="1">
+      <c r="B2" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="2:9" s="26" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B3" s="25"/>
-    </row>
-    <row r="4" spans="2:9" s="26" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-    </row>
-    <row r="5" spans="2:9" s="26" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B5" s="27" t="s">
+    <row r="3" spans="2:9" s="16" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B3" s="15"/>
+    </row>
+    <row r="4" spans="2:9" s="16" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="2:9" s="16" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-    </row>
-    <row r="6" spans="2:9" s="28" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B6" s="27"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-    </row>
-    <row r="7" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="30" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" s="18" customFormat="1" ht="13.5" customHeight="1">
+      <c r="B6" s="17"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="33">
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B8" s="22">
         <v>1</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="22">
         <v>0.1</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="22">
         <v>20140625</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="34" t="s">
+      <c r="F8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-    </row>
-    <row r="9" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B9" s="33">
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+    </row>
+    <row r="9" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B9" s="22">
         <v>2</v>
       </c>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-    </row>
-    <row r="10" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B10" s="33">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+    </row>
+    <row r="10" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B10" s="22">
         <v>3</v>
       </c>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-    </row>
-    <row r="11" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B11" s="33">
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+    </row>
+    <row r="11" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B11" s="22">
         <v>4</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-    </row>
-    <row r="12" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B12" s="33">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+    </row>
+    <row r="12" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B12" s="22">
         <v>5</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-    </row>
-    <row r="13" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B13" s="33">
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+    </row>
+    <row r="13" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B13" s="22">
         <v>6</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-    </row>
-    <row r="14" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B14" s="33">
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+    </row>
+    <row r="14" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B14" s="22">
         <v>7</v>
       </c>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B15" s="33">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+    </row>
+    <row r="15" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B15" s="22">
         <v>8</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-    </row>
-    <row r="16" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B16" s="33">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+    </row>
+    <row r="16" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B16" s="22">
         <v>9</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-    </row>
-    <row r="17" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B17" s="33">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+    </row>
+    <row r="17" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B17" s="22">
         <v>10</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="34"/>
-      <c r="G17" s="34"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-    </row>
-    <row r="18" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B18" s="33">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+    </row>
+    <row r="18" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B18" s="22">
         <v>11</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-    </row>
-    <row r="19" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B19" s="33">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+    </row>
+    <row r="19" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B19" s="22">
         <v>12</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-    </row>
-    <row r="20" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B20" s="33">
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+    </row>
+    <row r="20" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B20" s="22">
         <v>13</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-    </row>
-    <row r="21" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B21" s="33">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+    </row>
+    <row r="21" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B21" s="22">
         <v>14</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-    </row>
-    <row r="22" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B22" s="33">
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B22" s="22">
         <v>15</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-    </row>
-    <row r="23" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B23" s="33">
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+    </row>
+    <row r="23" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B23" s="22">
         <v>16</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-    </row>
-    <row r="24" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B24" s="33">
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+    </row>
+    <row r="24" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B24" s="22">
         <v>17</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
-    </row>
-    <row r="25" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B25" s="33">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+    </row>
+    <row r="25" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B25" s="22">
         <v>18</v>
       </c>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="34"/>
-      <c r="I25" s="34"/>
-    </row>
-    <row r="26" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B26" s="33">
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+    </row>
+    <row r="26" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B26" s="22">
         <v>19</v>
       </c>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
-      <c r="H26" s="34"/>
-      <c r="I26" s="34"/>
-    </row>
-    <row r="27" spans="2:9" s="32" customFormat="1" ht="15" customHeight="1">
-      <c r="B27" s="33">
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+    </row>
+    <row r="27" spans="2:9" s="21" customFormat="1" ht="15" customHeight="1">
+      <c r="B27" s="22">
         <v>20</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
     <mergeCell ref="F25:I25"/>
     <mergeCell ref="F26:I26"/>
     <mergeCell ref="F27:I27"/>
@@ -1350,21 +1379,10 @@
     <mergeCell ref="F22:I22"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F12:I12"/>
   </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31458333333333299" footer="0.31458333333333299"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L数据库结构一览表</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
@@ -1373,13 +1391,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:L231"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N17" sqref="N17"/>
+      <selection pane="bottomLeft" activeCell="G32" sqref="G32:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
@@ -1404,20 +1422,20 @@
       <c r="E2" s="11"/>
     </row>
     <row r="4" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19" t="s">
+      <c r="E4" s="32"/>
+      <c r="F4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="40" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="12" t="s">
@@ -1426,570 +1444,578 @@
       <c r="I4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="38" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B5" s="19"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="18"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="41"/>
       <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="24"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="38"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B6" s="20">
+      <c r="B6" s="28">
         <v>1</v>
       </c>
       <c r="C6" s="9">
         <v>41815</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="34"/>
+      <c r="F6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B7" s="21"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
     </row>
     <row r="8" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B8" s="20">
+      <c r="B8" s="28">
         <v>2</v>
       </c>
       <c r="C8" s="9">
         <v>41815</v>
       </c>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="15" t="s">
+      <c r="E8" s="34"/>
+      <c r="F8" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B9" s="21"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
     </row>
     <row r="10" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B10" s="20">
+      <c r="B10" s="28">
         <v>3</v>
       </c>
       <c r="C10" s="9">
         <v>41815</v>
       </c>
-      <c r="D10" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="26"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B11" s="21"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B12" s="20">
+      <c r="B12" s="28">
         <v>4</v>
       </c>
       <c r="C12" s="9">
         <v>41815</v>
       </c>
-      <c r="D12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="15" t="s">
+      <c r="D12" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B13" s="21"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
     </row>
     <row r="14" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B14" s="20">
+      <c r="B14" s="28">
         <v>5</v>
       </c>
       <c r="C14" s="9">
         <v>41815</v>
       </c>
-      <c r="D14" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="15" t="s">
+      <c r="D14" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="26"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B15" s="21"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
     </row>
     <row r="16" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B16" s="20">
+      <c r="B16" s="28">
         <v>6</v>
       </c>
       <c r="C16" s="9">
         <v>41815</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="22"/>
-      <c r="F16" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="G16" s="15"/>
+      <c r="D16" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="26"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B17" s="21"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="16"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B18" s="20">
+      <c r="B18" s="28">
         <v>7</v>
       </c>
       <c r="C18" s="9">
         <v>41815</v>
       </c>
-      <c r="D18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="22"/>
-      <c r="F18" s="15" t="s">
+      <c r="D18" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="15"/>
+      <c r="G18" s="26"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B19" s="21"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B20" s="20">
+      <c r="B20" s="28">
         <v>8</v>
       </c>
       <c r="C20" s="9">
         <v>41815</v>
       </c>
-      <c r="D20" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="22"/>
-      <c r="F20" s="15" t="s">
+      <c r="D20" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="30"/>
+      <c r="F20" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="15"/>
+      <c r="G20" s="26"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="21"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="16"/>
-      <c r="K21" s="16"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="20">
+      <c r="B22" s="28">
         <v>9</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
+      <c r="C22" s="9">
+        <v>41815</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="26"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="21"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="16"/>
-      <c r="K23" s="16"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B24" s="20">
+      <c r="B24" s="28">
         <v>10</v>
       </c>
       <c r="C24" s="9"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B25" s="21"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="16"/>
-      <c r="K25" s="16"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B26" s="20">
+      <c r="B26" s="28">
         <v>11</v>
       </c>
       <c r="C26" s="9"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="15"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B27" s="21"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="16"/>
-      <c r="K27" s="16"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
     </row>
     <row r="28" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B28" s="20">
+      <c r="B28" s="28">
         <v>12</v>
       </c>
       <c r="C28" s="9"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B29" s="21"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B30" s="20">
+      <c r="B30" s="28">
         <v>13</v>
       </c>
       <c r="C30" s="9"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
     </row>
     <row r="31" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B31" s="21"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B32" s="20">
+      <c r="B32" s="28">
         <v>14</v>
       </c>
       <c r="C32" s="9"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
     </row>
     <row r="33" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B33" s="21"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="16"/>
-      <c r="K33" s="16"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
     </row>
     <row r="34" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B34" s="20">
+      <c r="B34" s="28">
         <v>15</v>
       </c>
       <c r="C34" s="9"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B35" s="21"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
     </row>
     <row r="36" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B36" s="20">
+      <c r="B36" s="28">
         <v>16</v>
       </c>
       <c r="C36" s="9"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B37" s="21"/>
+      <c r="B37" s="29"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="16"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
     </row>
     <row r="38" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B38" s="20">
+      <c r="B38" s="28">
         <v>17</v>
       </c>
       <c r="C38" s="9"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
     </row>
     <row r="39" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B39" s="21"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
     </row>
     <row r="40" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B40" s="20">
+      <c r="B40" s="28">
         <v>18</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
     </row>
     <row r="41" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B41" s="21"/>
+      <c r="B41" s="29"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
-      <c r="J41" s="16"/>
-      <c r="K41" s="16"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" ht="13.5" customHeight="1">
       <c r="E42" s="4"/>
@@ -2563,87 +2589,14 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J12:J13"/>
     <mergeCell ref="K16:K17"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="D12:E13"/>
@@ -2668,22 +2621,95 @@
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="D14:E15"/>
     <mergeCell ref="K12:K13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="J16:J17"/>
     <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="J38:J39"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G35">
       <formula1>"对应不要,修改程序,需求变更,修改测试用例"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F35">
       <formula1>"高,中,低"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2697,7 +2723,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B39"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
@@ -2722,6 +2748,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update bug list @Author : Alex
</commit_message>
<xml_diff>
--- a/04 Test Case/故障对应报告.xlsx
+++ b/04 Test Case/故障对应报告.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3270" yWindow="-315" windowWidth="14310" windowHeight="9690" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="版本履历" sheetId="10" r:id="rId1"/>
@@ -21,12 +21,17 @@
     <definedName name="title" localSheetId="0">版本履历!$B$4:$I$5</definedName>
     <definedName name="title">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>完成时间</t>
   </si>
@@ -107,14 +112,7 @@
     <t>中</t>
   </si>
   <si>
-    <t>无错误处理页面，直接返回500和404错误
-404错误时，返回页面的连接无效</t>
-  </si>
-  <si>
     <t>Banner没有跑马灯效果</t>
-  </si>
-  <si>
-    <t>下载游戏页，点击图片没有全屏显示</t>
   </si>
   <si>
     <t>日志Logger wogamecenter_info.log 不准确</t>
@@ -126,6 +124,36 @@
   </si>
   <si>
     <t>有些游戏的图标没有显示出来</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>首页角标没有</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>首页栏目手势左右滑动</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>详情页下载按钮没有显示</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>详情页滑动时保留头部游戏名称</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>详情游戏页，点击图片没有全屏显示</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>搜索初始页面显示列表内容（参照沃游戏）</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>无错误处理页面，直接返回500和404错误
+404错误时，返回页面的连接无效
+公共错误页面处理，参照沃游戏。</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -137,7 +165,7 @@
     <numFmt numFmtId="176" formatCode="yy/m/d"/>
     <numFmt numFmtId="177" formatCode="yy/mm/dd"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <name val="ＭＳ 明朝"/>
@@ -228,8 +256,24 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="ＭＳ 明朝"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="ＭＳ 明朝"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +292,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -259,74 +315,74 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -334,41 +390,41 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -388,7 +444,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
@@ -397,8 +453,14 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -481,54 +543,75 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="10">
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="標準_Sheet1" xfId="3"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="9" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1358,6 +1441,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I8"/>
@@ -1370,46 +1462,42 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31458333333333299" footer="0.31458333333333299"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L数据库结构一览表</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5"/>
+  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
   <dimension ref="B1:L231"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G32" sqref="G32:G33"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.75" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" customWidth="1"/>
     <col min="3" max="4" width="9" style="2" customWidth="1"/>
     <col min="5" max="5" width="50.625" style="5" customWidth="1"/>
     <col min="6" max="9" width="9" style="3" customWidth="1"/>
-    <col min="10" max="11" width="9" style="2"/>
+    <col min="10" max="11" width="8.875" style="2"/>
     <col min="12" max="12" width="9" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="2"/>
+    <col min="13" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="19.5" customHeight="1">
@@ -1422,20 +1510,20 @@
       <c r="E2" s="11"/>
     </row>
     <row r="4" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="30" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32" t="s">
+      <c r="E4" s="30"/>
+      <c r="F4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="28" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="12" t="s">
@@ -1444,44 +1532,44 @@
       <c r="I4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="32" t="s">
+      <c r="J4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="31" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B5" s="32"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="41"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="38"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="31"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B6" s="28">
+      <c r="B6" s="32">
         <v>1</v>
       </c>
       <c r="C6" s="9">
         <v>41815</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="41"/>
       <c r="F6" s="26" t="s">
         <v>22</v>
       </c>
@@ -1493,12 +1581,12 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B7" s="29"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="36"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="8"/>
@@ -1507,16 +1595,16 @@
       <c r="K7" s="27"/>
     </row>
     <row r="8" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B8" s="28">
+      <c r="B8" s="32">
         <v>2</v>
       </c>
       <c r="C8" s="9">
         <v>41815</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="26" t="s">
         <v>22</v>
       </c>
@@ -1528,12 +1616,12 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B9" s="29"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="36"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="8"/>
@@ -1542,16 +1630,16 @@
       <c r="K9" s="27"/>
     </row>
     <row r="10" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B10" s="28">
+      <c r="B10" s="32">
         <v>3</v>
       </c>
       <c r="C10" s="9">
         <v>41815</v>
       </c>
       <c r="D10" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="30"/>
+        <v>28</v>
+      </c>
+      <c r="E10" s="34"/>
       <c r="F10" s="26" t="s">
         <v>22</v>
       </c>
@@ -1563,12 +1651,12 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B11" s="29"/>
+      <c r="B11" s="33"/>
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
       <c r="H11" s="8"/>
@@ -1577,16 +1665,16 @@
       <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B12" s="28">
+      <c r="B12" s="32">
         <v>4</v>
       </c>
       <c r="C12" s="9">
         <v>41815</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="34"/>
       <c r="F12" s="26" t="s">
         <v>22</v>
       </c>
@@ -1598,12 +1686,12 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B13" s="29"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="8"/>
@@ -1612,16 +1700,16 @@
       <c r="K13" s="27"/>
     </row>
     <row r="14" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B14" s="28">
+      <c r="B14" s="32">
         <v>5</v>
       </c>
       <c r="C14" s="9">
         <v>41815</v>
       </c>
-      <c r="D14" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="30"/>
+      <c r="D14" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="37"/>
       <c r="F14" s="26" t="s">
         <v>22</v>
       </c>
@@ -1632,13 +1720,13 @@
       <c r="K14" s="26"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B15" s="29"/>
+    <row r="15" spans="2:12" ht="25.5" customHeight="1">
+      <c r="B15" s="33"/>
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="8"/>
@@ -1647,16 +1735,16 @@
       <c r="K15" s="27"/>
     </row>
     <row r="16" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B16" s="28">
+      <c r="B16" s="32">
         <v>6</v>
       </c>
       <c r="C16" s="9">
         <v>41815</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="30"/>
+      <c r="D16" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="34"/>
       <c r="F16" s="26" t="s">
         <v>25</v>
       </c>
@@ -1668,12 +1756,12 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B17" s="29"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
       <c r="H17" s="8"/>
@@ -1682,16 +1770,16 @@
       <c r="K17" s="27"/>
     </row>
     <row r="18" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B18" s="28">
+      <c r="B18" s="32">
         <v>7</v>
       </c>
       <c r="C18" s="9">
         <v>41815</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="30"/>
+      <c r="D18" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="45"/>
       <c r="F18" s="26" t="s">
         <v>22</v>
       </c>
@@ -1702,12 +1790,12 @@
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B19" s="29"/>
+      <c r="B19" s="33"/>
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
       <c r="H19" s="8"/>
@@ -1716,16 +1804,16 @@
       <c r="K19" s="27"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B20" s="28">
+      <c r="B20" s="32">
         <v>8</v>
       </c>
       <c r="C20" s="9">
         <v>41815</v>
       </c>
-      <c r="D20" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="30"/>
+      <c r="D20" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="45"/>
       <c r="F20" s="26" t="s">
         <v>22</v>
       </c>
@@ -1736,12 +1824,12 @@
       <c r="K20" s="26"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="29"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="8"/>
@@ -1750,16 +1838,16 @@
       <c r="K21" s="27"/>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="28">
+      <c r="B22" s="32">
         <v>9</v>
       </c>
       <c r="C22" s="9">
         <v>41815</v>
       </c>
-      <c r="D22" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="30"/>
+      <c r="D22" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="34"/>
       <c r="F22" s="26" t="s">
         <v>22</v>
       </c>
@@ -1770,12 +1858,12 @@
       <c r="K22" s="26"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="29"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="8"/>
@@ -1784,13 +1872,19 @@
       <c r="K23" s="27"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B24" s="28">
+      <c r="B24" s="32">
         <v>10</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="26"/>
+      <c r="C24" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="45"/>
+      <c r="F24" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G24" s="26"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1798,10 +1892,12 @@
       <c r="K24" s="26"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B25" s="29"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="8"/>
@@ -1810,13 +1906,19 @@
       <c r="K25" s="27"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B26" s="28">
+      <c r="B26" s="32">
         <v>11</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="26"/>
+      <c r="C26" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G26" s="26"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1824,10 +1926,12 @@
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B27" s="29"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
       <c r="H27" s="8"/>
@@ -1836,13 +1940,19 @@
       <c r="K27" s="27"/>
     </row>
     <row r="28" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B28" s="28">
+      <c r="B28" s="32">
         <v>12</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="26"/>
+      <c r="C28" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="45"/>
+      <c r="F28" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G28" s="26"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -1850,10 +1960,12 @@
       <c r="K28" s="26"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B29" s="29"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
       <c r="H29" s="8"/>
@@ -1862,13 +1974,19 @@
       <c r="K29" s="27"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B30" s="28">
+      <c r="B30" s="32">
         <v>13</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="26"/>
+      <c r="C30" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D30" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" s="45"/>
+      <c r="F30" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G30" s="26"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -1876,10 +1994,12 @@
       <c r="K30" s="26"/>
     </row>
     <row r="31" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B31" s="29"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
       <c r="H31" s="8"/>
@@ -1888,13 +2008,19 @@
       <c r="K31" s="27"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B32" s="28">
+      <c r="B32" s="32">
         <v>14</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="26"/>
+      <c r="C32" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D32" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="45"/>
+      <c r="F32" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G32" s="26"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -1902,10 +2028,12 @@
       <c r="K32" s="26"/>
     </row>
     <row r="33" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B33" s="29"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
+      <c r="B33" s="33"/>
+      <c r="C33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27"/>
       <c r="H33" s="8"/>
@@ -1914,12 +2042,12 @@
       <c r="K33" s="27"/>
     </row>
     <row r="34" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B34" s="28">
+      <c r="B34" s="32">
         <v>15</v>
       </c>
       <c r="C34" s="9"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
       <c r="F34" s="26"/>
       <c r="G34" s="26"/>
       <c r="H34" s="6"/>
@@ -1928,10 +2056,10 @@
       <c r="K34" s="26"/>
     </row>
     <row r="35" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B35" s="29"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="46"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" s="8"/>
@@ -1940,12 +2068,12 @@
       <c r="K35" s="27"/>
     </row>
     <row r="36" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B36" s="28">
+      <c r="B36" s="32">
         <v>16</v>
       </c>
       <c r="C36" s="9"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
       <c r="F36" s="26"/>
       <c r="G36" s="26"/>
       <c r="H36" s="6"/>
@@ -1954,10 +2082,10 @@
       <c r="K36" s="26"/>
     </row>
     <row r="37" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B37" s="29"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
+      <c r="D37" s="46"/>
+      <c r="E37" s="46"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
       <c r="H37" s="8"/>
@@ -1966,12 +2094,12 @@
       <c r="K37" s="27"/>
     </row>
     <row r="38" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B38" s="28">
+      <c r="B38" s="32">
         <v>17</v>
       </c>
       <c r="C38" s="9"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
       <c r="H38" s="6"/>
@@ -1980,10 +2108,10 @@
       <c r="K38" s="26"/>
     </row>
     <row r="39" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B39" s="29"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
       <c r="H39" s="8"/>
@@ -1992,12 +2120,12 @@
       <c r="K39" s="27"/>
     </row>
     <row r="40" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B40" s="28">
+      <c r="B40" s="32">
         <v>18</v>
       </c>
       <c r="C40" s="9"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
       <c r="H40" s="6"/>
@@ -2006,10 +2134,10 @@
       <c r="K40" s="26"/>
     </row>
     <row r="41" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B41" s="29"/>
+      <c r="B41" s="33"/>
       <c r="C41" s="7"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
       <c r="H41" s="8"/>
@@ -2589,48 +2717,66 @@
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D4:E5"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="D14:E15"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D8:E9"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="J22:J23"/>
     <mergeCell ref="K18:K19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="D20:E21"/>
@@ -2643,66 +2789,48 @@
     <mergeCell ref="F18:F19"/>
     <mergeCell ref="G18:G19"/>
     <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="D28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J6:J7"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="2">
@@ -2714,11 +2842,16 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.62992125984251968" right="0.19685039370078741" top="0.74803149606299213" bottom="0.55118110236220474" header="0.47244094488188981" footer="0.19685039370078741"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L故障对应报告</oddHeader>
     <oddFooter>&amp;R&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2730,7 +2863,7 @@
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2">
@@ -2751,5 +2884,10 @@
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update Document @Author : Alex
</commit_message>
<xml_diff>
--- a/04 Test Case/故障对应报告.xlsx
+++ b/04 Test Case/故障对应报告.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22905"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="15560" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="版本履历" sheetId="10" r:id="rId1"/>
-    <sheet name="故障对应报告" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
+    <sheet name="沃游戏WAP端" sheetId="7" r:id="rId2"/>
+    <sheet name="沃游戏后台管理系统" sheetId="12" r:id="rId3"/>
+    <sheet name="附件" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">故障对应报告!$B$15:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">沃游戏WAP端!$B$15:$I$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">沃游戏后台管理系统!$B$15:$I$15</definedName>
     <definedName name="createtime">版本履历!$E$4:$F$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">沃游戏WAP端!$A$1:$I$17</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">沃游戏后台管理系统!$A$1:$I$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">版本履历!$A$2:J34</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">故障对应报告!$A$1:$I$17</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">故障对应报告!$4:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">沃游戏WAP端!$4:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">沃游戏后台管理系统!$4:$5</definedName>
     <definedName name="project">版本履历!$B$4:$B$5</definedName>
+    <definedName name="title" localSheetId="2">#REF!</definedName>
     <definedName name="title" localSheetId="0">版本履历!$B$4:$I$5</definedName>
     <definedName name="title">#REF!</definedName>
   </definedNames>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="47">
   <si>
     <t>完成时间</t>
   </si>
@@ -131,10 +136,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>首页栏目手势左右滑动</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>详情页下载按钮没有显示</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -147,25 +148,65 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>搜索初始页面显示列表内容（参照沃游戏）</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>无错误处理页面，直接返回500和404错误
 404错误时，返回页面的连接无效
 公共错误页面处理，参照沃游戏。</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>分类详情标题显示乱码，其对应的游戏无下载按钮</t>
+  </si>
+  <si>
+    <t>手机上点击下载按钮无效</t>
+  </si>
+  <si>
+    <t>搜索初始页面显示列表内容（参照沃游戏）</t>
+  </si>
+  <si>
+    <t>游戏详情页的搜索按钮无效</t>
+  </si>
+  <si>
+    <t>首页栏目手势左右滑动，且滑动时页面不要出现余白。</t>
+  </si>
+  <si>
+    <t>首页的Banner没有点击的效果</t>
+  </si>
+  <si>
+    <t>详情页的下载按钮显示出来了【编号15】，但游戏的介绍图片不见了</t>
+  </si>
+  <si>
+    <t>Task：日志分析Job</t>
+  </si>
+  <si>
+    <t>Task：中兴多渠道下载回执文件分析Job</t>
+  </si>
+  <si>
+    <t>登录页面“记住我的登录账号”没做</t>
+  </si>
+  <si>
+    <t>日志总览页
+1.日数据和月数据联动
+2.higtcharts显示图片
+3.31省分公司进入该页面
+4.左侧的菜单无效</t>
+  </si>
+  <si>
+    <t>建站管理页
+1.建站详情CSS调整
+2.点击已启用的Site按钮没有变灰
+3.页面“已建站点详情”上有多个“C”
+4.左侧“日志总览”无效</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yy/m/d"/>
-    <numFmt numFmtId="177" formatCode="yy/mm/dd"/>
+    <numFmt numFmtId="164" formatCode="yy/m/d"/>
+    <numFmt numFmtId="165" formatCode="yy/mm/dd"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <name val="ＭＳ 明朝"/>
@@ -273,7 +314,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,7 +507,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -480,13 +527,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -498,10 +545,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -543,6 +590,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,68 +645,44 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="標準_Sheet1" xfId="3"/>
-    <cellStyle name="常规 2" xfId="1"/>
-    <cellStyle name="超链接" xfId="4" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="6" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="8" builtinId="8" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1116,21 +1187,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:I27"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="23" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="23" customWidth="1"/>
     <col min="2" max="2" width="6" style="23" customWidth="1"/>
     <col min="3" max="3" width="8" style="23" customWidth="1"/>
     <col min="4" max="4" width="10" style="23" customWidth="1"/>
     <col min="5" max="9" width="8" style="23" customWidth="1"/>
-    <col min="10" max="10" width="1.6640625" style="23" customWidth="1"/>
+    <col min="10" max="10" width="1.625" style="23" customWidth="1"/>
     <col min="11" max="12" width="8" style="23" customWidth="1"/>
     <col min="13" max="16384" width="8" style="23"/>
   </cols>
@@ -1441,15 +1512,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="F19:I19"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
     <mergeCell ref="F18:I18"/>
     <mergeCell ref="F7:I7"/>
     <mergeCell ref="F8:I8"/>
@@ -1462,6 +1524,15 @@
     <mergeCell ref="F15:I15"/>
     <mergeCell ref="F16:I16"/>
     <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.31458333333333299" footer="0.31458333333333299"/>
@@ -1479,25 +1550,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
-  <dimension ref="B1:L231"/>
+  <dimension ref="B1:L261"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20:E21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="9" style="3" customWidth="1"/>
     <col min="3" max="4" width="9" style="2" customWidth="1"/>
-    <col min="5" max="5" width="50.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="50.625" style="5" customWidth="1"/>
     <col min="6" max="9" width="9" style="3" customWidth="1"/>
-    <col min="10" max="11" width="8.83203125" style="2"/>
+    <col min="10" max="11" width="8.875" style="2"/>
     <col min="12" max="12" width="9" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.83203125" style="2"/>
+    <col min="13" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="19.5" customHeight="1">
@@ -1510,20 +1581,20 @@
       <c r="E2" s="11"/>
     </row>
     <row r="4" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="34" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30" t="s">
+      <c r="E4" s="34"/>
+      <c r="F4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="44" t="s">
         <v>15</v>
       </c>
       <c r="H4" s="12" t="s">
@@ -1532,44 +1603,44 @@
       <c r="I4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="30" t="s">
+      <c r="J4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="K4" s="46" t="s">
         <v>16</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B5" s="30"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="29"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="45"/>
       <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="J5" s="30"/>
-      <c r="K5" s="35"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="46"/>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B6" s="31">
+      <c r="B6" s="28">
         <v>1</v>
       </c>
       <c r="C6" s="9">
         <v>41815</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="40"/>
       <c r="F6" s="26" t="s">
         <v>22</v>
       </c>
@@ -1581,12 +1652,12 @@
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B7" s="32"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="38"/>
-      <c r="E7" s="39"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
       <c r="F7" s="27"/>
       <c r="G7" s="27"/>
       <c r="H7" s="8"/>
@@ -1595,16 +1666,16 @@
       <c r="K7" s="27"/>
     </row>
     <row r="8" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B8" s="31">
+      <c r="B8" s="28">
         <v>2</v>
       </c>
       <c r="C8" s="9">
         <v>41815</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="37"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="26" t="s">
         <v>22</v>
       </c>
@@ -1616,12 +1687,12 @@
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B9" s="32"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="27"/>
       <c r="G9" s="27"/>
       <c r="H9" s="8"/>
@@ -1630,16 +1701,16 @@
       <c r="K9" s="27"/>
     </row>
     <row r="10" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B10" s="31">
+      <c r="B10" s="28">
         <v>3</v>
       </c>
       <c r="C10" s="9">
         <v>41815</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="40"/>
+      <c r="E10" s="32"/>
       <c r="F10" s="26" t="s">
         <v>22</v>
       </c>
@@ -1651,12 +1722,12 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B11" s="32"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="27"/>
       <c r="G11" s="27"/>
       <c r="H11" s="8"/>
@@ -1665,16 +1736,16 @@
       <c r="K11" s="27"/>
     </row>
     <row r="12" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B12" s="31">
+      <c r="B12" s="28">
         <v>4</v>
       </c>
       <c r="C12" s="9">
         <v>41815</v>
       </c>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="40"/>
+      <c r="E12" s="32"/>
       <c r="F12" s="26" t="s">
         <v>22</v>
       </c>
@@ -1686,12 +1757,12 @@
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B13" s="32"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="8"/>
@@ -1700,16 +1771,16 @@
       <c r="K13" s="27"/>
     </row>
     <row r="14" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B14" s="31">
+      <c r="B14" s="28">
         <v>5</v>
       </c>
       <c r="C14" s="9">
         <v>41815</v>
       </c>
-      <c r="D14" s="43" t="s">
-        <v>36</v>
-      </c>
-      <c r="E14" s="44"/>
+      <c r="D14" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="36"/>
       <c r="F14" s="26" t="s">
         <v>22</v>
       </c>
@@ -1720,13 +1791,13 @@
       <c r="K14" s="26"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B15" s="32"/>
+    <row r="15" spans="2:12" ht="28.5" customHeight="1">
+      <c r="B15" s="29"/>
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="8"/>
@@ -1735,16 +1806,16 @@
       <c r="K15" s="27"/>
     </row>
     <row r="16" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B16" s="31">
+      <c r="B16" s="28">
         <v>6</v>
       </c>
       <c r="C16" s="9">
         <v>41815</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="40"/>
+      <c r="E16" s="32"/>
       <c r="F16" s="26" t="s">
         <v>25</v>
       </c>
@@ -1756,12 +1827,12 @@
       <c r="L16" s="1"/>
     </row>
     <row r="17" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B17" s="32"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="27"/>
       <c r="G17" s="27"/>
       <c r="H17" s="8"/>
@@ -1770,16 +1841,16 @@
       <c r="K17" s="27"/>
     </row>
     <row r="18" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B18" s="31">
+      <c r="B18" s="28">
         <v>7</v>
       </c>
       <c r="C18" s="9">
         <v>41815</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="33"/>
+      <c r="D18" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="30"/>
       <c r="F18" s="26" t="s">
         <v>22</v>
       </c>
@@ -1790,12 +1861,12 @@
       <c r="K18" s="26"/>
     </row>
     <row r="19" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B19" s="32"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
       <c r="F19" s="27"/>
       <c r="G19" s="27"/>
       <c r="H19" s="8"/>
@@ -1804,16 +1875,16 @@
       <c r="K19" s="27"/>
     </row>
     <row r="20" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B20" s="31">
+      <c r="B20" s="28">
         <v>8</v>
       </c>
       <c r="C20" s="9">
         <v>41815</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="33"/>
+      <c r="E20" s="30"/>
       <c r="F20" s="26" t="s">
         <v>22</v>
       </c>
@@ -1824,12 +1895,12 @@
       <c r="K20" s="26"/>
     </row>
     <row r="21" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B21" s="32"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="27"/>
       <c r="G21" s="27"/>
       <c r="H21" s="8"/>
@@ -1838,16 +1909,16 @@
       <c r="K21" s="27"/>
     </row>
     <row r="22" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B22" s="31">
+      <c r="B22" s="28">
         <v>9</v>
       </c>
       <c r="C22" s="9">
         <v>41815</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="40"/>
+      <c r="E22" s="32"/>
       <c r="F22" s="26" t="s">
         <v>22</v>
       </c>
@@ -1858,12 +1929,12 @@
       <c r="K22" s="26"/>
     </row>
     <row r="23" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B23" s="32"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="8"/>
@@ -1872,17 +1943,19 @@
       <c r="K23" s="27"/>
     </row>
     <row r="24" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B24" s="31">
+      <c r="B24" s="28">
         <v>10</v>
       </c>
       <c r="C24" s="9">
         <v>41816</v>
       </c>
-      <c r="D24" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="26"/>
+      <c r="D24" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="32"/>
+      <c r="F24" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G24" s="26"/>
       <c r="H24" s="6"/>
       <c r="I24" s="6"/>
@@ -1890,12 +1963,12 @@
       <c r="K24" s="26"/>
     </row>
     <row r="25" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B25" s="32"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
       <c r="F25" s="27"/>
       <c r="G25" s="27"/>
       <c r="H25" s="8"/>
@@ -1904,17 +1977,19 @@
       <c r="K25" s="27"/>
     </row>
     <row r="26" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B26" s="31">
+      <c r="B26" s="28">
         <v>11</v>
       </c>
       <c r="C26" s="9">
         <v>41816</v>
       </c>
-      <c r="D26" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="26"/>
+      <c r="D26" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="32"/>
+      <c r="F26" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G26" s="26"/>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
@@ -1922,12 +1997,12 @@
       <c r="K26" s="26"/>
     </row>
     <row r="27" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B27" s="32"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
       <c r="F27" s="27"/>
       <c r="G27" s="27"/>
       <c r="H27" s="8"/>
@@ -1936,17 +2011,19 @@
       <c r="K27" s="27"/>
     </row>
     <row r="28" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B28" s="31">
+      <c r="B28" s="28">
         <v>12</v>
       </c>
       <c r="C28" s="9">
         <v>41816</v>
       </c>
-      <c r="D28" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="26"/>
+      <c r="D28" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="32"/>
+      <c r="F28" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G28" s="26"/>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -1954,12 +2031,12 @@
       <c r="K28" s="26"/>
     </row>
     <row r="29" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B29" s="32"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
       <c r="F29" s="27"/>
       <c r="G29" s="27"/>
       <c r="H29" s="8"/>
@@ -1968,17 +2045,19 @@
       <c r="K29" s="27"/>
     </row>
     <row r="30" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B30" s="31">
+      <c r="B30" s="28">
         <v>13</v>
       </c>
       <c r="C30" s="9">
         <v>41816</v>
       </c>
-      <c r="D30" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="26"/>
+      <c r="D30" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G30" s="26"/>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
@@ -1986,12 +2065,12 @@
       <c r="K30" s="26"/>
     </row>
     <row r="31" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B31" s="32"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="34"/>
-      <c r="E31" s="34"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
       <c r="F31" s="27"/>
       <c r="G31" s="27"/>
       <c r="H31" s="8"/>
@@ -2000,17 +2079,19 @@
       <c r="K31" s="27"/>
     </row>
     <row r="32" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B32" s="31">
+      <c r="B32" s="28">
         <v>14</v>
       </c>
       <c r="C32" s="9">
         <v>41816</v>
       </c>
-      <c r="D32" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="26"/>
+      <c r="D32" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32" s="30"/>
+      <c r="F32" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G32" s="26"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
@@ -2018,12 +2099,12 @@
       <c r="K32" s="26"/>
     </row>
     <row r="33" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B33" s="32"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="27"/>
       <c r="G33" s="27"/>
       <c r="H33" s="8"/>
@@ -2032,13 +2113,19 @@
       <c r="K33" s="27"/>
     </row>
     <row r="34" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B34" s="31">
+      <c r="B34" s="28">
         <v>15</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="26"/>
+      <c r="C34" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D34" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="30"/>
+      <c r="F34" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G34" s="26"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2046,10 +2133,12 @@
       <c r="K34" s="26"/>
     </row>
     <row r="35" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B35" s="32"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
       <c r="F35" s="27"/>
       <c r="G35" s="27"/>
       <c r="H35" s="8"/>
@@ -2058,13 +2147,19 @@
       <c r="K35" s="27"/>
     </row>
     <row r="36" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B36" s="31">
+      <c r="B36" s="28">
         <v>16</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="26"/>
+      <c r="C36" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G36" s="26"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2072,10 +2167,12 @@
       <c r="K36" s="26"/>
     </row>
     <row r="37" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B37" s="32"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="34"/>
-      <c r="E37" s="34"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
       <c r="F37" s="27"/>
       <c r="G37" s="27"/>
       <c r="H37" s="8"/>
@@ -2084,13 +2181,19 @@
       <c r="K37" s="27"/>
     </row>
     <row r="38" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B38" s="31">
+      <c r="B38" s="28">
         <v>17</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="26"/>
+      <c r="C38" s="9">
+        <v>41816</v>
+      </c>
+      <c r="D38" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="30"/>
+      <c r="F38" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G38" s="26"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2098,10 +2201,12 @@
       <c r="K38" s="26"/>
     </row>
     <row r="39" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B39" s="32"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="34"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
       <c r="F39" s="27"/>
       <c r="G39" s="27"/>
       <c r="H39" s="8"/>
@@ -2110,13 +2215,19 @@
       <c r="K39" s="27"/>
     </row>
     <row r="40" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B40" s="31">
+      <c r="B40" s="28">
         <v>18</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="26"/>
+      <c r="C40" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D40" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="30"/>
+      <c r="F40" s="26" t="s">
+        <v>22</v>
+      </c>
       <c r="G40" s="26"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -2124,10 +2235,12 @@
       <c r="K40" s="26"/>
     </row>
     <row r="41" spans="2:11" ht="13.5" customHeight="1">
-      <c r="B41" s="32"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="34"/>
-      <c r="E41" s="34"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
       <c r="F41" s="27"/>
       <c r="G41" s="27"/>
       <c r="H41" s="8"/>
@@ -2136,120 +2249,428 @@
       <c r="K41" s="27"/>
     </row>
     <row r="42" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E42" s="4"/>
+      <c r="B42" s="28">
+        <v>19</v>
+      </c>
+      <c r="C42" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E42" s="30"/>
+      <c r="F42" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G42" s="26"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
     </row>
     <row r="43" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E43" s="4"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
     </row>
     <row r="44" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E44" s="4"/>
+      <c r="B44" s="28">
+        <v>20</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
     </row>
     <row r="45" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E45" s="4"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
     </row>
     <row r="46" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E46" s="4"/>
+      <c r="B46" s="28">
+        <v>21</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
     </row>
     <row r="47" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E47" s="4"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
     </row>
     <row r="48" spans="2:11" ht="13.5" customHeight="1">
-      <c r="E48" s="4"/>
-    </row>
-    <row r="49" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E49" s="4"/>
-    </row>
-    <row r="50" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E51" s="4"/>
-    </row>
-    <row r="52" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E54" s="4"/>
-    </row>
-    <row r="55" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E55" s="4"/>
-    </row>
-    <row r="56" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E56" s="4"/>
-    </row>
-    <row r="57" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E58" s="4"/>
-    </row>
-    <row r="59" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E59" s="4"/>
-    </row>
-    <row r="60" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E61" s="4"/>
-    </row>
-    <row r="62" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E63" s="4"/>
-    </row>
-    <row r="64" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E64" s="4"/>
-    </row>
-    <row r="65" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E65" s="4"/>
-    </row>
-    <row r="66" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E66" s="4"/>
-    </row>
-    <row r="67" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E67" s="4"/>
-    </row>
-    <row r="68" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E68" s="4"/>
-    </row>
-    <row r="69" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E69" s="4"/>
-    </row>
-    <row r="70" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E70" s="4"/>
-    </row>
-    <row r="71" spans="5:5" ht="13.5" customHeight="1">
-      <c r="E71" s="4"/>
-    </row>
-    <row r="72" spans="5:5" ht="13.5" customHeight="1">
+      <c r="B48" s="28">
+        <v>22</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+    </row>
+    <row r="49" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B49" s="29"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+    </row>
+    <row r="50" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B50" s="28">
+        <v>23</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+    </row>
+    <row r="51" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B51" s="29"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+    </row>
+    <row r="52" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B52" s="28">
+        <v>24</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+    </row>
+    <row r="53" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B53" s="29"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+    </row>
+    <row r="54" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B54" s="28">
+        <v>25</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+    </row>
+    <row r="55" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B55" s="29"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+    </row>
+    <row r="56" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B56" s="28">
+        <v>26</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B57" s="29"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+    </row>
+    <row r="58" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B58" s="28">
+        <v>27</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+    </row>
+    <row r="59" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B59" s="29"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="27"/>
+      <c r="K59" s="27"/>
+    </row>
+    <row r="60" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B60" s="28">
+        <v>28</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+    </row>
+    <row r="61" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B61" s="29"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+    </row>
+    <row r="62" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B62" s="28">
+        <v>29</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+    </row>
+    <row r="63" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B63" s="29"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="27"/>
+    </row>
+    <row r="64" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B64" s="28">
+        <v>30</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+    </row>
+    <row r="65" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B65" s="29"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+    </row>
+    <row r="66" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B66" s="28">
+        <v>31</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26"/>
+    </row>
+    <row r="67" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B67" s="29"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+    </row>
+    <row r="68" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B68" s="28">
+        <v>32</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26"/>
+    </row>
+    <row r="69" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B69" s="29"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+    </row>
+    <row r="70" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B70" s="28">
+        <v>33</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+    </row>
+    <row r="71" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B71" s="29"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="27"/>
+      <c r="K71" s="27"/>
+    </row>
+    <row r="72" spans="2:11" ht="13.5" customHeight="1">
       <c r="E72" s="4"/>
     </row>
-    <row r="73" spans="5:5" ht="13.5" customHeight="1">
+    <row r="73" spans="2:11" ht="13.5" customHeight="1">
       <c r="E73" s="4"/>
     </row>
-    <row r="74" spans="5:5" ht="13.5" customHeight="1">
+    <row r="74" spans="2:11" ht="13.5" customHeight="1">
       <c r="E74" s="4"/>
     </row>
-    <row r="75" spans="5:5" ht="13.5" customHeight="1">
+    <row r="75" spans="2:11" ht="13.5" customHeight="1">
       <c r="E75" s="4"/>
     </row>
-    <row r="76" spans="5:5" ht="13.5" customHeight="1">
+    <row r="76" spans="2:11" ht="13.5" customHeight="1">
       <c r="E76" s="4"/>
     </row>
-    <row r="77" spans="5:5" ht="13.5" customHeight="1">
+    <row r="77" spans="2:11" ht="13.5" customHeight="1">
       <c r="E77" s="4"/>
     </row>
-    <row r="78" spans="5:5" ht="13.5" customHeight="1">
+    <row r="78" spans="2:11" ht="13.5" customHeight="1">
       <c r="E78" s="4"/>
     </row>
-    <row r="79" spans="5:5" ht="13.5" customHeight="1">
+    <row r="79" spans="2:11" ht="13.5" customHeight="1">
       <c r="E79" s="4"/>
     </row>
-    <row r="80" spans="5:5" ht="13.5" customHeight="1">
+    <row r="80" spans="2:11" ht="13.5" customHeight="1">
       <c r="E80" s="4"/>
     </row>
     <row r="81" spans="5:5" ht="13.5" customHeight="1">
@@ -2705,80 +3126,185 @@
     <row r="231" spans="5:5" ht="13.5" customHeight="1">
       <c r="E231" s="4"/>
     </row>
+    <row r="232" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E232" s="4"/>
+    </row>
+    <row r="233" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E233" s="4"/>
+    </row>
+    <row r="234" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E234" s="4"/>
+    </row>
+    <row r="235" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E235" s="4"/>
+    </row>
+    <row r="236" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E236" s="4"/>
+    </row>
+    <row r="237" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E237" s="4"/>
+    </row>
+    <row r="238" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E238" s="4"/>
+    </row>
+    <row r="239" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E239" s="4"/>
+    </row>
+    <row r="240" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E240" s="4"/>
+    </row>
+    <row r="241" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E241" s="4"/>
+    </row>
+    <row r="242" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E242" s="4"/>
+    </row>
+    <row r="243" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E243" s="4"/>
+    </row>
+    <row r="244" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E244" s="4"/>
+    </row>
+    <row r="245" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E245" s="4"/>
+    </row>
+    <row r="246" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E246" s="4"/>
+    </row>
+    <row r="247" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E247" s="4"/>
+    </row>
+    <row r="248" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E248" s="4"/>
+    </row>
+    <row r="249" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E249" s="4"/>
+    </row>
+    <row r="250" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E250" s="4"/>
+    </row>
+    <row r="251" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E251" s="4"/>
+    </row>
+    <row r="252" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E252" s="4"/>
+    </row>
+    <row r="253" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E253" s="4"/>
+    </row>
+    <row r="254" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E254" s="4"/>
+    </row>
+    <row r="255" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E255" s="4"/>
+    </row>
+    <row r="256" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E256" s="4"/>
+    </row>
+    <row r="257" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E257" s="4"/>
+    </row>
+    <row r="258" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E258" s="4"/>
+    </row>
+    <row r="259" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E259" s="4"/>
+    </row>
+    <row r="260" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E260" s="4"/>
+    </row>
+    <row r="261" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E261" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="114">
-    <mergeCell ref="K38:K39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="K40:K41"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:E39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="J38:J39"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="G36:G37"/>
-    <mergeCell ref="J36:J37"/>
-    <mergeCell ref="K36:K37"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D34:E35"/>
-    <mergeCell ref="F34:F35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="J34:J35"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="D32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="K26:K27"/>
+  <mergeCells count="204">
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="D28:E29"/>
     <mergeCell ref="F28:F29"/>
     <mergeCell ref="G28:G29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="K28:K29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="D26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="D24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="D20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="D66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="K66:K67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="K64:K65"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="D60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="K54:K55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="D56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="K56:K57"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="D50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="J6:J7"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="D12:E13"/>
     <mergeCell ref="F12:F13"/>
@@ -2800,34 +3326,109 @@
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="D8:E9"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="D70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="K48:K49"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G71">
       <formula1>"对应不要,修改程序,需求变更,修改测试用例"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F71">
       <formula1>"高,中,低"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2846,14 +3447,1792 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:L261"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="1.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9" style="3" customWidth="1"/>
+    <col min="3" max="4" width="9" style="2" customWidth="1"/>
+    <col min="5" max="5" width="50.625" style="5" customWidth="1"/>
+    <col min="6" max="9" width="9" style="3" customWidth="1"/>
+    <col min="10" max="11" width="8.875" style="2"/>
+    <col min="12" max="12" width="9" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="19.5" customHeight="1">
+      <c r="B1" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B2" s="11"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="4" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B5" s="34"/>
+      <c r="C5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="34"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B6" s="28">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="48"/>
+      <c r="F6" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B7" s="29"/>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="49"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+    </row>
+    <row r="8" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B8" s="28">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="48"/>
+      <c r="F8" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="26"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B9" s="29"/>
+      <c r="C9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="49"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+    </row>
+    <row r="10" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B10" s="28">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="53"/>
+      <c r="F10" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B11" s="29"/>
+      <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+    </row>
+    <row r="12" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B12" s="28">
+        <v>4</v>
+      </c>
+      <c r="C12" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D12" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="53"/>
+      <c r="F12" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="26"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="2:12" ht="51" customHeight="1">
+      <c r="B13" s="29"/>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+    </row>
+    <row r="14" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B14" s="28">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9">
+        <v>41820</v>
+      </c>
+      <c r="D14" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="53"/>
+      <c r="F14" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="26"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="2:12" ht="56.25" customHeight="1">
+      <c r="B15" s="29"/>
+      <c r="C15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+    </row>
+    <row r="16" spans="2:12" ht="13.5" customHeight="1">
+      <c r="B16" s="28">
+        <v>6</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B17" s="29"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+    </row>
+    <row r="18" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B18" s="28">
+        <v>7</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="26"/>
+      <c r="K18" s="26"/>
+    </row>
+    <row r="19" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B19" s="29"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+    </row>
+    <row r="20" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B20" s="28">
+        <v>8</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B21" s="29"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+    </row>
+    <row r="22" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B22" s="28">
+        <v>9</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+    </row>
+    <row r="23" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B23" s="29"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+    </row>
+    <row r="24" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B24" s="28">
+        <v>15</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+    </row>
+    <row r="25" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B25" s="29"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+    </row>
+    <row r="26" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B26" s="28">
+        <v>16</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+    </row>
+    <row r="27" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B27" s="29"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+    </row>
+    <row r="28" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B28" s="28">
+        <v>17</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+    </row>
+    <row r="29" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B29" s="29"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+    </row>
+    <row r="30" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B30" s="28">
+        <v>10</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+    </row>
+    <row r="31" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B31" s="29"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+    </row>
+    <row r="32" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B32" s="28">
+        <v>11</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+    </row>
+    <row r="33" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B33" s="29"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="54"/>
+      <c r="E33" s="54"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="27"/>
+      <c r="K33" s="27"/>
+    </row>
+    <row r="34" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B34" s="28">
+        <v>12</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="26"/>
+    </row>
+    <row r="35" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B35" s="29"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="54"/>
+      <c r="E35" s="54"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+    </row>
+    <row r="36" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B36" s="28">
+        <v>13</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B37" s="29"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+    </row>
+    <row r="38" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B38" s="28">
+        <v>14</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+    </row>
+    <row r="39" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B39" s="29"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+    </row>
+    <row r="40" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B40" s="28">
+        <v>15</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+    </row>
+    <row r="41" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B41" s="29"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="27"/>
+    </row>
+    <row r="42" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B42" s="28">
+        <v>16</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+    </row>
+    <row r="43" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B43" s="29"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+    </row>
+    <row r="44" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B44" s="28">
+        <v>17</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+    </row>
+    <row r="45" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B45" s="29"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+    </row>
+    <row r="46" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B46" s="28">
+        <v>18</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+    </row>
+    <row r="47" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B47" s="29"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
+    </row>
+    <row r="48" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B48" s="28">
+        <v>19</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="26"/>
+    </row>
+    <row r="49" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B49" s="29"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="27"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="27"/>
+    </row>
+    <row r="50" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B50" s="28">
+        <v>20</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="26"/>
+      <c r="K50" s="26"/>
+    </row>
+    <row r="51" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B51" s="29"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+    </row>
+    <row r="52" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B52" s="28">
+        <v>21</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="26"/>
+      <c r="K52" s="26"/>
+    </row>
+    <row r="53" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B53" s="29"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+    </row>
+    <row r="54" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B54" s="28">
+        <v>22</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="26"/>
+      <c r="G54" s="26"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="26"/>
+      <c r="K54" s="26"/>
+    </row>
+    <row r="55" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B55" s="29"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+    </row>
+    <row r="56" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B56" s="28">
+        <v>23</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="26"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="26"/>
+    </row>
+    <row r="57" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B57" s="29"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+    </row>
+    <row r="58" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B58" s="28">
+        <v>24</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="30"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="26"/>
+      <c r="G58" s="26"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="26"/>
+    </row>
+    <row r="59" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B59" s="29"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="27"/>
+      <c r="K59" s="27"/>
+    </row>
+    <row r="60" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B60" s="28">
+        <v>25</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="30"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="26"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="26"/>
+    </row>
+    <row r="61" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B61" s="29"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="31"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="27"/>
+      <c r="K61" s="27"/>
+    </row>
+    <row r="62" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B62" s="28">
+        <v>26</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="26"/>
+      <c r="K62" s="26"/>
+    </row>
+    <row r="63" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B63" s="29"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="31"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="27"/>
+      <c r="G63" s="27"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="27"/>
+      <c r="K63" s="27"/>
+    </row>
+    <row r="64" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B64" s="28">
+        <v>27</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="26"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="26"/>
+      <c r="K64" s="26"/>
+    </row>
+    <row r="65" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B65" s="29"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="31"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="27"/>
+      <c r="G65" s="27"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="27"/>
+      <c r="K65" s="27"/>
+    </row>
+    <row r="66" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B66" s="28">
+        <v>28</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="26"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="26"/>
+      <c r="K66" s="26"/>
+    </row>
+    <row r="67" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B67" s="29"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="27"/>
+      <c r="G67" s="27"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="27"/>
+      <c r="K67" s="27"/>
+    </row>
+    <row r="68" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B68" s="28">
+        <v>29</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="30"/>
+      <c r="E68" s="30"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="26"/>
+      <c r="K68" s="26"/>
+    </row>
+    <row r="69" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B69" s="29"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="27"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+    </row>
+    <row r="70" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B70" s="28">
+        <v>30</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="30"/>
+      <c r="E70" s="30"/>
+      <c r="F70" s="26"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="26"/>
+    </row>
+    <row r="71" spans="2:11" ht="13.5" customHeight="1">
+      <c r="B71" s="29"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="27"/>
+      <c r="G71" s="27"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="27"/>
+      <c r="K71" s="27"/>
+    </row>
+    <row r="72" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E72" s="4"/>
+    </row>
+    <row r="73" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E73" s="4"/>
+    </row>
+    <row r="74" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E74" s="4"/>
+    </row>
+    <row r="75" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E75" s="4"/>
+    </row>
+    <row r="76" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E76" s="4"/>
+    </row>
+    <row r="77" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E77" s="4"/>
+    </row>
+    <row r="78" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E78" s="4"/>
+    </row>
+    <row r="79" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E79" s="4"/>
+    </row>
+    <row r="80" spans="2:11" ht="13.5" customHeight="1">
+      <c r="E80" s="4"/>
+    </row>
+    <row r="81" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E81" s="4"/>
+    </row>
+    <row r="82" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E82" s="4"/>
+    </row>
+    <row r="83" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E83" s="4"/>
+    </row>
+    <row r="84" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E84" s="4"/>
+    </row>
+    <row r="85" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E85" s="4"/>
+    </row>
+    <row r="86" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E86" s="4"/>
+    </row>
+    <row r="87" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E87" s="4"/>
+    </row>
+    <row r="88" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E88" s="4"/>
+    </row>
+    <row r="89" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E89" s="4"/>
+    </row>
+    <row r="90" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E90" s="4"/>
+    </row>
+    <row r="91" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E91" s="4"/>
+    </row>
+    <row r="92" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E92" s="4"/>
+    </row>
+    <row r="93" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E93" s="4"/>
+    </row>
+    <row r="94" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E94" s="4"/>
+    </row>
+    <row r="95" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E95" s="4"/>
+    </row>
+    <row r="96" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E96" s="4"/>
+    </row>
+    <row r="97" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E97" s="4"/>
+    </row>
+    <row r="98" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E98" s="4"/>
+    </row>
+    <row r="99" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E99" s="4"/>
+    </row>
+    <row r="100" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E100" s="4"/>
+    </row>
+    <row r="101" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E101" s="4"/>
+    </row>
+    <row r="102" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E102" s="4"/>
+    </row>
+    <row r="103" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E103" s="4"/>
+    </row>
+    <row r="104" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E104" s="4"/>
+    </row>
+    <row r="105" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E105" s="4"/>
+    </row>
+    <row r="106" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E106" s="4"/>
+    </row>
+    <row r="107" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E107" s="4"/>
+    </row>
+    <row r="108" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E108" s="4"/>
+    </row>
+    <row r="109" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E109" s="4"/>
+    </row>
+    <row r="110" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E110" s="4"/>
+    </row>
+    <row r="111" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E111" s="4"/>
+    </row>
+    <row r="112" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E112" s="4"/>
+    </row>
+    <row r="113" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E113" s="4"/>
+    </row>
+    <row r="114" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E114" s="4"/>
+    </row>
+    <row r="115" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E115" s="4"/>
+    </row>
+    <row r="116" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E116" s="4"/>
+    </row>
+    <row r="117" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E117" s="4"/>
+    </row>
+    <row r="118" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E118" s="4"/>
+    </row>
+    <row r="119" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E119" s="4"/>
+    </row>
+    <row r="120" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E120" s="4"/>
+    </row>
+    <row r="121" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E121" s="4"/>
+    </row>
+    <row r="122" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E122" s="4"/>
+    </row>
+    <row r="123" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E123" s="4"/>
+    </row>
+    <row r="124" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E124" s="4"/>
+    </row>
+    <row r="125" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E125" s="4"/>
+    </row>
+    <row r="126" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E126" s="4"/>
+    </row>
+    <row r="127" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E127" s="4"/>
+    </row>
+    <row r="128" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E128" s="4"/>
+    </row>
+    <row r="129" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E129" s="4"/>
+    </row>
+    <row r="130" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E130" s="4"/>
+    </row>
+    <row r="131" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E131" s="4"/>
+    </row>
+    <row r="132" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E132" s="4"/>
+    </row>
+    <row r="133" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E133" s="4"/>
+    </row>
+    <row r="134" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E134" s="4"/>
+    </row>
+    <row r="135" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E135" s="4"/>
+    </row>
+    <row r="136" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E136" s="4"/>
+    </row>
+    <row r="137" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E137" s="4"/>
+    </row>
+    <row r="138" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E138" s="4"/>
+    </row>
+    <row r="139" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E139" s="4"/>
+    </row>
+    <row r="140" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E140" s="4"/>
+    </row>
+    <row r="141" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E141" s="4"/>
+    </row>
+    <row r="142" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E142" s="4"/>
+    </row>
+    <row r="143" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E143" s="4"/>
+    </row>
+    <row r="144" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E144" s="4"/>
+    </row>
+    <row r="145" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E145" s="4"/>
+    </row>
+    <row r="146" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E146" s="4"/>
+    </row>
+    <row r="147" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E147" s="4"/>
+    </row>
+    <row r="148" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E148" s="4"/>
+    </row>
+    <row r="149" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E149" s="4"/>
+    </row>
+    <row r="150" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E150" s="4"/>
+    </row>
+    <row r="151" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E151" s="4"/>
+    </row>
+    <row r="152" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E152" s="4"/>
+    </row>
+    <row r="153" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E153" s="4"/>
+    </row>
+    <row r="154" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E154" s="4"/>
+    </row>
+    <row r="155" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E155" s="4"/>
+    </row>
+    <row r="156" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E156" s="4"/>
+    </row>
+    <row r="157" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E157" s="4"/>
+    </row>
+    <row r="158" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E158" s="4"/>
+    </row>
+    <row r="159" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E159" s="4"/>
+    </row>
+    <row r="160" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E160" s="4"/>
+    </row>
+    <row r="161" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E161" s="4"/>
+    </row>
+    <row r="162" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E162" s="4"/>
+    </row>
+    <row r="163" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E163" s="4"/>
+    </row>
+    <row r="164" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E164" s="4"/>
+    </row>
+    <row r="165" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E165" s="4"/>
+    </row>
+    <row r="166" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E166" s="4"/>
+    </row>
+    <row r="167" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E167" s="4"/>
+    </row>
+    <row r="168" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E168" s="4"/>
+    </row>
+    <row r="169" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E169" s="4"/>
+    </row>
+    <row r="170" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E170" s="4"/>
+    </row>
+    <row r="171" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E171" s="4"/>
+    </row>
+    <row r="172" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E172" s="4"/>
+    </row>
+    <row r="173" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E173" s="4"/>
+    </row>
+    <row r="174" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E174" s="4"/>
+    </row>
+    <row r="175" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E175" s="4"/>
+    </row>
+    <row r="176" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E176" s="4"/>
+    </row>
+    <row r="177" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E177" s="4"/>
+    </row>
+    <row r="178" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E178" s="4"/>
+    </row>
+    <row r="179" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E179" s="4"/>
+    </row>
+    <row r="180" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E180" s="4"/>
+    </row>
+    <row r="181" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E181" s="4"/>
+    </row>
+    <row r="182" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E182" s="4"/>
+    </row>
+    <row r="183" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E183" s="4"/>
+    </row>
+    <row r="184" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E184" s="4"/>
+    </row>
+    <row r="185" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E185" s="4"/>
+    </row>
+    <row r="186" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E186" s="4"/>
+    </row>
+    <row r="187" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E187" s="4"/>
+    </row>
+    <row r="188" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E188" s="4"/>
+    </row>
+    <row r="189" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E189" s="4"/>
+    </row>
+    <row r="190" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E190" s="4"/>
+    </row>
+    <row r="191" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E191" s="4"/>
+    </row>
+    <row r="192" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E192" s="4"/>
+    </row>
+    <row r="193" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E193" s="4"/>
+    </row>
+    <row r="194" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E194" s="4"/>
+    </row>
+    <row r="195" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E195" s="4"/>
+    </row>
+    <row r="196" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E196" s="4"/>
+    </row>
+    <row r="197" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E197" s="4"/>
+    </row>
+    <row r="198" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E198" s="4"/>
+    </row>
+    <row r="199" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E199" s="4"/>
+    </row>
+    <row r="200" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E200" s="4"/>
+    </row>
+    <row r="201" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E201" s="4"/>
+    </row>
+    <row r="202" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E202" s="4"/>
+    </row>
+    <row r="203" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E203" s="4"/>
+    </row>
+    <row r="204" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E204" s="4"/>
+    </row>
+    <row r="205" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E205" s="4"/>
+    </row>
+    <row r="206" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E206" s="4"/>
+    </row>
+    <row r="207" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E207" s="4"/>
+    </row>
+    <row r="208" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E208" s="4"/>
+    </row>
+    <row r="209" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E209" s="4"/>
+    </row>
+    <row r="210" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E210" s="4"/>
+    </row>
+    <row r="211" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E211" s="4"/>
+    </row>
+    <row r="212" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E212" s="4"/>
+    </row>
+    <row r="213" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E213" s="4"/>
+    </row>
+    <row r="214" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E214" s="4"/>
+    </row>
+    <row r="215" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E215" s="4"/>
+    </row>
+    <row r="216" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E216" s="4"/>
+    </row>
+    <row r="217" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E217" s="4"/>
+    </row>
+    <row r="218" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E218" s="4"/>
+    </row>
+    <row r="219" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E219" s="4"/>
+    </row>
+    <row r="220" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E220" s="4"/>
+    </row>
+    <row r="221" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E221" s="4"/>
+    </row>
+    <row r="222" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E222" s="4"/>
+    </row>
+    <row r="223" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E223" s="4"/>
+    </row>
+    <row r="224" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E224" s="4"/>
+    </row>
+    <row r="225" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E225" s="4"/>
+    </row>
+    <row r="226" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E226" s="4"/>
+    </row>
+    <row r="227" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E227" s="4"/>
+    </row>
+    <row r="228" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E228" s="4"/>
+    </row>
+    <row r="229" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E229" s="4"/>
+    </row>
+    <row r="230" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E230" s="4"/>
+    </row>
+    <row r="231" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E231" s="4"/>
+    </row>
+    <row r="232" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E232" s="4"/>
+    </row>
+    <row r="233" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E233" s="4"/>
+    </row>
+    <row r="234" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E234" s="4"/>
+    </row>
+    <row r="235" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E235" s="4"/>
+    </row>
+    <row r="236" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E236" s="4"/>
+    </row>
+    <row r="237" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E237" s="4"/>
+    </row>
+    <row r="238" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E238" s="4"/>
+    </row>
+    <row r="239" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E239" s="4"/>
+    </row>
+    <row r="240" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E240" s="4"/>
+    </row>
+    <row r="241" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E241" s="4"/>
+    </row>
+    <row r="242" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E242" s="4"/>
+    </row>
+    <row r="243" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E243" s="4"/>
+    </row>
+    <row r="244" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E244" s="4"/>
+    </row>
+    <row r="245" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E245" s="4"/>
+    </row>
+    <row r="246" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E246" s="4"/>
+    </row>
+    <row r="247" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E247" s="4"/>
+    </row>
+    <row r="248" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E248" s="4"/>
+    </row>
+    <row r="249" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E249" s="4"/>
+    </row>
+    <row r="250" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E250" s="4"/>
+    </row>
+    <row r="251" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E251" s="4"/>
+    </row>
+    <row r="252" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E252" s="4"/>
+    </row>
+    <row r="253" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E253" s="4"/>
+    </row>
+    <row r="254" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E254" s="4"/>
+    </row>
+    <row r="255" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E255" s="4"/>
+    </row>
+    <row r="256" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E256" s="4"/>
+    </row>
+    <row r="257" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E257" s="4"/>
+    </row>
+    <row r="258" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E258" s="4"/>
+    </row>
+    <row r="259" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E259" s="4"/>
+    </row>
+    <row r="260" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E260" s="4"/>
+    </row>
+    <row r="261" spans="5:5" ht="13.5" customHeight="1">
+      <c r="E261" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="204">
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="D70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="D66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="K66:K67"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="K64:K65"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="D60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="D58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="D56:E57"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="K56:K57"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="D54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="K54:K55"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="D52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="K52:K53"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="D50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:E49"/>
+    <mergeCell ref="F48:F49"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="K48:K49"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="J46:J47"/>
+    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="J42:J43"/>
+    <mergeCell ref="K42:K43"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="J40:J41"/>
+    <mergeCell ref="K40:K41"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:E39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="J38:J39"/>
+    <mergeCell ref="K38:K39"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="K36:K37"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="D34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="D26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="D22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="D20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="D8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
+  </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F71">
+      <formula1>"高,中,低"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G71">
+      <formula1>"对应不要,修改程序,需求变更,修改测试用例"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.62992125984251968" right="0.19685039370078741" top="0.74803149606299213" bottom="0.55118110236220474" header="0.47244094488188981" footer="0.19685039370078741"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;L故障对应报告</oddHeader>
+    <oddFooter>&amp;R&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:B39"/>
   <sheetViews>
     <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="I64" sqref="I64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2">

</xml_diff>